<commit_message>
java syllabus updated and dummy file got added
</commit_message>
<xml_diff>
--- a/Java Syallabus.xlsx
+++ b/Java Syallabus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\OJT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1819D157-4B18-4A68-9838-D0F15B5AC8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9FD6D-5562-47A4-A4B6-8200F7FFE635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C69188D5-3413-42BD-A72B-0245F13F4DB4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
   <si>
     <t>Introduction</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>Check Constraints</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BAA9CE-78D4-4DF4-8779-B5CE08C693AB}">
   <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,6 +1335,9 @@
       <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>